<commit_message>
added sample entry to report template
</commit_message>
<xml_diff>
--- a/storage/app/public/report-template.xlsx
+++ b/storage/app/public/report-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\XAMPP\htdocs\carbon-dash\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\XAMPP\htdocs\carbon-dash\storage\app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03CEB761-CFA8-4A0A-A405-F0C9E96F3F8D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAEC6FD-2A03-4E24-8A80-D358D8CA1E3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Plate Number</t>
   </si>
@@ -44,6 +44,18 @@
   <si>
     <t>Requesting Department</t>
   </si>
+  <si>
+    <t>August 22, 2018</t>
+  </si>
+  <si>
+    <t>Sample Department</t>
+  </si>
+  <si>
+    <t>ABC123</t>
+  </si>
+  <si>
+    <t>Sample Destination</t>
+  </si>
 </sst>
 </file>
 
@@ -54,7 +66,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="#,##0.00;[Red]#,##0.00"/>
     <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="170" formatCode="[$-3409]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="168" formatCode="[$-3409]dd\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -112,7 +124,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -168,10 +180,13 @@
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -490,13 +505,13 @@
   <dimension ref="A1:I186"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="25" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="17" style="25" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="29" customWidth="1"/>
     <col min="3" max="3" width="18" style="14" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" style="15" customWidth="1"/>
     <col min="5" max="5" width="30.7109375" style="6" customWidth="1"/>
@@ -511,7 +526,7 @@
       <c r="A1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="26" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="13" t="s">
@@ -528,28 +543,42 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="24"/>
+      <c r="A2" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="15">
+        <v>100</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="24">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="H2" s="7"/>
       <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="8"/>
       <c r="E3" s="12"/>
       <c r="H3" s="7"/>
       <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="7"/>
+      <c r="B4" s="27"/>
       <c r="E4" s="9"/>
       <c r="H4" s="7"/>
       <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="8"/>
       <c r="E5" s="9"/>
       <c r="F5" s="24"/>
@@ -557,7 +586,7 @@
       <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="8"/>
       <c r="E6" s="9"/>
       <c r="F6" s="22"/>
@@ -565,14 +594,14 @@
       <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="8"/>
       <c r="E7" s="9"/>
       <c r="H7" s="7"/>
       <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B8" s="7"/>
+      <c r="B8" s="27"/>
       <c r="E8" s="9"/>
       <c r="G8" s="3"/>
     </row>
@@ -582,32 +611,32 @@
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B10" s="10"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="8"/>
       <c r="E10" s="9"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B11" s="10"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="8"/>
       <c r="E11" s="9"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B12" s="7"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="8"/>
       <c r="E12" s="9"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B13" s="10"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="8"/>
       <c r="E13" s="9"/>
       <c r="F13" s="22"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="8"/>
       <c r="E14" s="9"/>
       <c r="F14" s="24"/>
@@ -615,7 +644,7 @@
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B15" s="7"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="11"/>
       <c r="D15" s="16"/>
       <c r="E15" s="9"/>
@@ -623,7 +652,7 @@
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B16" s="7"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="8"/>
       <c r="D16" s="17"/>
       <c r="E16" s="12"/>
@@ -631,14 +660,14 @@
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="8"/>
       <c r="D17" s="16"/>
       <c r="E17" s="9"/>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="11"/>
       <c r="D18" s="16"/>
       <c r="E18" s="9"/>
@@ -651,7 +680,7 @@
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="11"/>
       <c r="D20" s="16"/>
       <c r="E20" s="9"/>
@@ -664,7 +693,7 @@
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
+      <c r="B22" s="27"/>
       <c r="C22" s="8"/>
       <c r="D22" s="16"/>
       <c r="E22" s="9"/>
@@ -674,37 +703,37 @@
       <c r="C23" s="11"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
+      <c r="B24" s="27"/>
       <c r="D24" s="17"/>
       <c r="E24" s="12"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
+      <c r="B25" s="27"/>
       <c r="C25" s="8"/>
       <c r="I25" s="18"/>
     </row>
     <row r="26" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B26" s="7"/>
+      <c r="B26" s="27"/>
       <c r="C26" s="11"/>
       <c r="D26" s="16"/>
       <c r="E26" s="9"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B27" s="7"/>
+      <c r="B27" s="27"/>
       <c r="D27" s="16"/>
       <c r="E27" s="9"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B28" s="10"/>
+      <c r="B28" s="28"/>
       <c r="C28" s="8"/>
       <c r="D28" s="16"/>
       <c r="E28" s="9"/>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="11"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -712,26 +741,26 @@
       <c r="E30" s="9"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
+      <c r="B31" s="27"/>
       <c r="C31" s="8"/>
       <c r="D31" s="16"/>
       <c r="E31" s="9"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="10"/>
+      <c r="B32" s="28"/>
       <c r="C32" s="8"/>
       <c r="D32" s="16"/>
       <c r="E32" s="9"/>
     </row>
     <row r="33" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B33" s="7"/>
+      <c r="B33" s="27"/>
       <c r="C33" s="8"/>
       <c r="D33" s="16"/>
       <c r="E33" s="9"/>
       <c r="G33" s="3"/>
     </row>
     <row r="34" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B34" s="7"/>
+      <c r="B34" s="27"/>
       <c r="D34" s="16"/>
       <c r="E34" s="9"/>
       <c r="G34" s="3"/>
@@ -743,7 +772,7 @@
       <c r="G35" s="3"/>
     </row>
     <row r="36" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B36" s="7"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="8"/>
       <c r="D36" s="16"/>
       <c r="E36" s="9"/>
@@ -755,14 +784,14 @@
       <c r="G37" s="3"/>
     </row>
     <row r="38" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B38" s="7"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="8"/>
       <c r="D38" s="16"/>
       <c r="F38" s="22"/>
       <c r="G38" s="3"/>
     </row>
     <row r="39" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B39" s="10"/>
+      <c r="B39" s="28"/>
       <c r="C39" s="8"/>
       <c r="D39" s="16"/>
       <c r="E39" s="9"/>
@@ -770,7 +799,7 @@
       <c r="G39" s="3"/>
     </row>
     <row r="40" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B40" s="7"/>
+      <c r="B40" s="27"/>
       <c r="C40" s="8"/>
       <c r="D40" s="16"/>
       <c r="E40" s="9"/>
@@ -781,33 +810,33 @@
       <c r="F41" s="22"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="7"/>
+      <c r="B42" s="27"/>
       <c r="C42" s="8"/>
       <c r="E42" s="12"/>
       <c r="F42" s="22"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="7"/>
+      <c r="B43" s="27"/>
       <c r="E43" s="9"/>
       <c r="F43" s="22"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="7"/>
+      <c r="B44" s="27"/>
       <c r="E44" s="9"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="10"/>
+      <c r="B45" s="28"/>
       <c r="C45" s="8"/>
       <c r="E45" s="9"/>
     </row>
     <row r="46" spans="2:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B46" s="7"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="11"/>
       <c r="E46" s="9"/>
       <c r="G46" s="4"/>
     </row>
     <row r="47" spans="2:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B47" s="7"/>
+      <c r="B47" s="27"/>
       <c r="C47" s="8"/>
       <c r="D47" s="17"/>
       <c r="E47" s="12"/>
@@ -820,31 +849,31 @@
       <c r="G48" s="4"/>
     </row>
     <row r="49" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B49" s="7"/>
+      <c r="B49" s="27"/>
       <c r="C49" s="8"/>
       <c r="F49" s="23"/>
       <c r="G49" s="4"/>
     </row>
     <row r="50" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B50" s="7"/>
+      <c r="B50" s="27"/>
       <c r="C50" s="8"/>
       <c r="E50" s="9"/>
       <c r="F50" s="22"/>
       <c r="G50" s="4"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="10"/>
+      <c r="B51" s="28"/>
       <c r="C51" s="8"/>
       <c r="E51" s="9"/>
       <c r="F51" s="24"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="7"/>
+      <c r="B52" s="27"/>
       <c r="C52" s="8"/>
       <c r="E52" s="12"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B53" s="7"/>
+      <c r="B53" s="27"/>
       <c r="C53" s="8"/>
       <c r="E53" s="9"/>
     </row>
@@ -852,7 +881,7 @@
       <c r="E54" s="9"/>
     </row>
     <row r="55" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B55" s="7"/>
+      <c r="B55" s="27"/>
       <c r="C55" s="8"/>
       <c r="D55" s="16"/>
       <c r="E55" s="9"/>
@@ -860,7 +889,7 @@
       <c r="G55" s="4"/>
     </row>
     <row r="56" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B56" s="7"/>
+      <c r="B56" s="27"/>
       <c r="C56" s="8"/>
       <c r="D56" s="16"/>
       <c r="E56" s="9"/>
@@ -868,7 +897,7 @@
       <c r="G56" s="4"/>
     </row>
     <row r="57" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B57" s="7"/>
+      <c r="B57" s="27"/>
       <c r="C57" s="8"/>
       <c r="D57" s="16"/>
       <c r="E57" s="9"/>
@@ -883,14 +912,14 @@
       <c r="I58" s="3"/>
     </row>
     <row r="59" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B59" s="10"/>
+      <c r="B59" s="28"/>
       <c r="D59" s="16"/>
       <c r="E59" s="12"/>
       <c r="G59" s="4"/>
       <c r="I59" s="3"/>
     </row>
     <row r="60" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B60" s="10"/>
+      <c r="B60" s="28"/>
       <c r="C60" s="8"/>
       <c r="D60" s="16"/>
       <c r="E60" s="9"/>
@@ -898,7 +927,7 @@
       <c r="I60" s="3"/>
     </row>
     <row r="61" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B61" s="10"/>
+      <c r="B61" s="28"/>
       <c r="C61" s="11"/>
       <c r="D61" s="16"/>
       <c r="E61" s="9"/>
@@ -906,26 +935,26 @@
       <c r="I61" s="3"/>
     </row>
     <row r="62" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B62" s="10"/>
+      <c r="B62" s="28"/>
       <c r="C62" s="8"/>
       <c r="D62" s="17"/>
       <c r="E62" s="9"/>
       <c r="G62" s="4"/>
     </row>
     <row r="63" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B63" s="10"/>
+      <c r="B63" s="28"/>
       <c r="C63" s="8"/>
       <c r="D63" s="16"/>
       <c r="E63" s="12"/>
       <c r="G63" s="4"/>
     </row>
     <row r="64" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B64" s="7"/>
+      <c r="B64" s="27"/>
       <c r="E64" s="9"/>
       <c r="G64" s="4"/>
     </row>
     <row r="65" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B65" s="7"/>
+      <c r="B65" s="27"/>
       <c r="C65" s="11"/>
       <c r="E65" s="12"/>
       <c r="G65" s="4"/>
@@ -937,14 +966,14 @@
       <c r="I66" s="3"/>
     </row>
     <row r="67" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B67" s="7"/>
+      <c r="B67" s="27"/>
       <c r="C67" s="11"/>
       <c r="F67" s="22"/>
       <c r="G67" s="4"/>
       <c r="I67" s="3"/>
     </row>
     <row r="68" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B68" s="10"/>
+      <c r="B68" s="28"/>
       <c r="C68" s="8"/>
       <c r="D68" s="16"/>
       <c r="E68" s="9"/>
@@ -952,7 +981,7 @@
       <c r="G68" s="4"/>
     </row>
     <row r="69" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B69" s="7"/>
+      <c r="B69" s="27"/>
       <c r="C69" s="8"/>
       <c r="D69" s="16"/>
       <c r="E69" s="9"/>
@@ -960,27 +989,27 @@
       <c r="G69" s="4"/>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B70" s="7"/>
+      <c r="B70" s="27"/>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C71" s="8"/>
       <c r="E71" s="9"/>
     </row>
     <row r="72" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B72" s="7"/>
+      <c r="B72" s="27"/>
       <c r="C72" s="8"/>
       <c r="D72" s="16"/>
       <c r="E72" s="9"/>
       <c r="G72" s="3"/>
     </row>
     <row r="73" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B73" s="10"/>
+      <c r="B73" s="28"/>
       <c r="D73" s="16"/>
       <c r="E73" s="9"/>
       <c r="G73" s="3"/>
     </row>
     <row r="74" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B74" s="7"/>
+      <c r="B74" s="27"/>
       <c r="C74" s="8"/>
       <c r="D74" s="16"/>
       <c r="E74" s="9"/>
@@ -988,48 +1017,48 @@
       <c r="G74" s="3"/>
     </row>
     <row r="75" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B75" s="10"/>
+      <c r="B75" s="28"/>
       <c r="C75" s="8"/>
       <c r="D75" s="16"/>
       <c r="E75" s="9"/>
       <c r="G75" s="3"/>
     </row>
     <row r="76" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B76" s="7"/>
+      <c r="B76" s="27"/>
       <c r="C76" s="8"/>
       <c r="E76" s="9"/>
       <c r="G76" s="3"/>
     </row>
     <row r="77" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B77" s="7"/>
+      <c r="B77" s="27"/>
       <c r="C77" s="8"/>
       <c r="G77" s="3"/>
     </row>
     <row r="78" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B78" s="7"/>
+      <c r="B78" s="27"/>
       <c r="C78" s="8"/>
       <c r="E78" s="9"/>
       <c r="G78" s="3"/>
     </row>
     <row r="79" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B79" s="7"/>
+      <c r="B79" s="27"/>
       <c r="E79" s="9"/>
       <c r="G79" s="3"/>
     </row>
     <row r="80" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B80" s="7"/>
+      <c r="B80" s="27"/>
       <c r="C80" s="11"/>
       <c r="G80" s="3"/>
     </row>
     <row r="81" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B81" s="10"/>
+      <c r="B81" s="28"/>
       <c r="C81" s="8"/>
       <c r="E81" s="9"/>
       <c r="F81" s="22"/>
       <c r="G81" s="3"/>
     </row>
     <row r="82" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B82" s="7"/>
+      <c r="B82" s="27"/>
       <c r="C82" s="8"/>
       <c r="E82" s="9"/>
       <c r="F82" s="22"/>
@@ -1042,57 +1071,57 @@
       <c r="G83" s="3"/>
     </row>
     <row r="84" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B84" s="7"/>
+      <c r="B84" s="27"/>
       <c r="C84" s="8"/>
       <c r="E84" s="9"/>
       <c r="G84" s="3"/>
     </row>
     <row r="85" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B85" s="10"/>
+      <c r="B85" s="28"/>
       <c r="E85" s="12"/>
       <c r="G85" s="3"/>
     </row>
     <row r="86" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B86" s="7"/>
+      <c r="B86" s="27"/>
       <c r="C86" s="8"/>
       <c r="E86" s="9"/>
       <c r="F86" s="24"/>
       <c r="G86" s="3"/>
     </row>
     <row r="87" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B87" s="10"/>
+      <c r="B87" s="28"/>
       <c r="C87" s="8"/>
       <c r="E87" s="9"/>
       <c r="F87" s="22"/>
       <c r="G87" s="3"/>
     </row>
     <row r="88" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B88" s="7"/>
+      <c r="B88" s="27"/>
       <c r="C88" s="8"/>
       <c r="E88" s="9"/>
       <c r="G88" s="3"/>
     </row>
     <row r="89" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B89" s="7"/>
+      <c r="B89" s="27"/>
       <c r="D89" s="16"/>
       <c r="E89" s="9"/>
       <c r="G89" s="3"/>
     </row>
     <row r="90" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B90" s="10"/>
+      <c r="B90" s="28"/>
       <c r="C90" s="8"/>
       <c r="E90" s="9"/>
       <c r="G90" s="3"/>
     </row>
     <row r="91" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B91" s="7"/>
+      <c r="B91" s="27"/>
       <c r="C91" s="8"/>
       <c r="D91" s="16"/>
       <c r="E91" s="9"/>
       <c r="G91" s="3"/>
     </row>
     <row r="92" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B92" s="7"/>
+      <c r="B92" s="27"/>
       <c r="E92" s="9"/>
       <c r="G92" s="3"/>
     </row>
@@ -1101,19 +1130,19 @@
       <c r="G93" s="3"/>
     </row>
     <row r="94" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B94" s="7"/>
+      <c r="B94" s="27"/>
       <c r="E94" s="9"/>
       <c r="F94" s="22"/>
       <c r="G94" s="3"/>
     </row>
     <row r="95" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B95" s="7"/>
+      <c r="B95" s="27"/>
       <c r="C95" s="8"/>
       <c r="F95" s="24"/>
       <c r="G95" s="3"/>
     </row>
     <row r="96" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B96" s="7"/>
+      <c r="B96" s="27"/>
       <c r="C96" s="8"/>
       <c r="E96" s="9"/>
       <c r="G96" s="3"/>
@@ -1123,7 +1152,7 @@
       <c r="G97" s="3"/>
     </row>
     <row r="98" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B98" s="7"/>
+      <c r="B98" s="27"/>
       <c r="C98" s="8"/>
       <c r="E98" s="9"/>
       <c r="G98" s="4"/>
@@ -1136,7 +1165,7 @@
       <c r="G99" s="4"/>
     </row>
     <row r="100" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B100" s="7"/>
+      <c r="B100" s="27"/>
       <c r="C100" s="8"/>
       <c r="D100" s="16"/>
       <c r="E100" s="9"/>
@@ -1144,7 +1173,7 @@
       <c r="G100" s="4"/>
     </row>
     <row r="101" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B101" s="7"/>
+      <c r="B101" s="27"/>
       <c r="C101" s="8"/>
       <c r="D101" s="17"/>
       <c r="E101" s="9"/>
@@ -1152,7 +1181,7 @@
       <c r="G101" s="4"/>
     </row>
     <row r="102" spans="2:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B102" s="7"/>
+      <c r="B102" s="27"/>
       <c r="C102" s="8"/>
       <c r="D102" s="16"/>
       <c r="G102" s="4"/>
@@ -1171,7 +1200,7 @@
       <c r="I104" s="5"/>
     </row>
     <row r="105" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B105" s="7"/>
+      <c r="B105" s="27"/>
       <c r="C105" s="8"/>
       <c r="D105" s="17"/>
       <c r="E105" s="9"/>
@@ -1179,14 +1208,14 @@
       <c r="I105" s="5"/>
     </row>
     <row r="106" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B106" s="7"/>
+      <c r="B106" s="27"/>
       <c r="C106" s="8"/>
       <c r="E106" s="9"/>
       <c r="G106" s="3"/>
       <c r="I106" s="5"/>
     </row>
     <row r="107" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B107" s="7"/>
+      <c r="B107" s="27"/>
       <c r="C107" s="8"/>
       <c r="D107" s="17"/>
       <c r="E107" s="9"/>
@@ -1201,7 +1230,7 @@
       <c r="I108" s="5"/>
     </row>
     <row r="109" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B109" s="7"/>
+      <c r="B109" s="27"/>
       <c r="D109" s="16"/>
       <c r="E109" s="9"/>
       <c r="F109" s="24"/>
@@ -1209,7 +1238,7 @@
       <c r="I109" s="5"/>
     </row>
     <row r="110" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B110" s="7"/>
+      <c r="B110" s="27"/>
       <c r="C110" s="8"/>
       <c r="D110" s="16"/>
       <c r="F110" s="24"/>
@@ -1217,7 +1246,7 @@
       <c r="I110" s="5"/>
     </row>
     <row r="111" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B111" s="10"/>
+      <c r="B111" s="28"/>
       <c r="C111" s="8"/>
       <c r="D111" s="17"/>
       <c r="E111" s="9"/>
@@ -1225,7 +1254,7 @@
       <c r="I111" s="5"/>
     </row>
     <row r="112" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B112" s="7"/>
+      <c r="B112" s="27"/>
       <c r="C112" s="8"/>
       <c r="D112" s="16"/>
       <c r="E112" s="12"/>
@@ -1247,7 +1276,7 @@
       <c r="I114" s="5"/>
     </row>
     <row r="115" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B115" s="7"/>
+      <c r="B115" s="27"/>
       <c r="C115" s="8"/>
       <c r="D115" s="16"/>
       <c r="E115" s="9"/>
@@ -1256,7 +1285,7 @@
       <c r="I115" s="5"/>
     </row>
     <row r="116" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B116" s="7"/>
+      <c r="B116" s="27"/>
       <c r="C116" s="8"/>
       <c r="D116" s="16"/>
       <c r="E116" s="9"/>
@@ -1265,7 +1294,7 @@
       <c r="I116" s="5"/>
     </row>
     <row r="117" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B117" s="7"/>
+      <c r="B117" s="27"/>
       <c r="D117" s="16"/>
       <c r="E117" s="9"/>
       <c r="F117" s="24"/>
@@ -1280,7 +1309,7 @@
       <c r="I118" s="5"/>
     </row>
     <row r="119" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B119" s="10"/>
+      <c r="B119" s="28"/>
       <c r="C119" s="8"/>
       <c r="D119" s="16"/>
       <c r="E119" s="9"/>
@@ -1288,7 +1317,7 @@
       <c r="I119" s="5"/>
     </row>
     <row r="120" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B120" s="7"/>
+      <c r="B120" s="27"/>
       <c r="C120" s="8"/>
       <c r="D120" s="16"/>
       <c r="E120" s="12"/>
@@ -1296,7 +1325,7 @@
       <c r="I120" s="5"/>
     </row>
     <row r="121" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B121" s="7"/>
+      <c r="B121" s="27"/>
       <c r="D121" s="16"/>
       <c r="E121" s="9"/>
       <c r="F121" s="24"/>
@@ -1304,7 +1333,7 @@
       <c r="I121" s="5"/>
     </row>
     <row r="122" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B122" s="10"/>
+      <c r="B122" s="28"/>
       <c r="C122" s="8"/>
       <c r="D122" s="16"/>
       <c r="E122" s="9"/>
@@ -1313,7 +1342,7 @@
       <c r="I122" s="5"/>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B123" s="7"/>
+      <c r="B123" s="27"/>
       <c r="E123" s="9"/>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.25">
@@ -1321,43 +1350,43 @@
       <c r="E124" s="9"/>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B125" s="7"/>
+      <c r="B125" s="27"/>
       <c r="C125" s="8"/>
       <c r="D125" s="16"/>
       <c r="E125" s="9"/>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B126" s="10"/>
+      <c r="B126" s="28"/>
       <c r="D126" s="16"/>
       <c r="E126" s="9"/>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B127" s="7"/>
+      <c r="B127" s="27"/>
       <c r="D127" s="17"/>
       <c r="E127" s="9"/>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B128" s="10"/>
+      <c r="B128" s="28"/>
       <c r="C128" s="8"/>
       <c r="D128" s="16"/>
       <c r="E128" s="9"/>
       <c r="F128" s="22"/>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B129" s="10"/>
+      <c r="B129" s="28"/>
       <c r="C129" s="8"/>
       <c r="D129" s="17"/>
       <c r="E129" s="9"/>
       <c r="F129" s="24"/>
     </row>
     <row r="130" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B130" s="7"/>
+      <c r="B130" s="27"/>
       <c r="C130" s="8"/>
       <c r="D130" s="16"/>
       <c r="E130" s="12"/>
     </row>
     <row r="131" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B131" s="10"/>
+      <c r="B131" s="28"/>
       <c r="C131" s="8"/>
       <c r="E131" s="9"/>
     </row>
@@ -1365,53 +1394,53 @@
       <c r="E132" s="9"/>
     </row>
     <row r="133" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B133" s="10"/>
+      <c r="B133" s="28"/>
       <c r="C133" s="8"/>
       <c r="E133" s="12"/>
       <c r="F133" s="24"/>
     </row>
     <row r="134" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B134" s="7"/>
+      <c r="B134" s="27"/>
       <c r="D134" s="17"/>
       <c r="E134" s="9"/>
     </row>
     <row r="135" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B135" s="10"/>
+      <c r="B135" s="28"/>
       <c r="C135" s="8"/>
       <c r="D135" s="17"/>
       <c r="E135" s="9"/>
     </row>
     <row r="136" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B136" s="7"/>
+      <c r="B136" s="27"/>
       <c r="C136" s="8"/>
       <c r="E136" s="9"/>
     </row>
     <row r="137" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B137" s="7"/>
+      <c r="B137" s="27"/>
       <c r="C137" s="8"/>
       <c r="E137" s="9"/>
     </row>
     <row r="138" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B138" s="7"/>
+      <c r="B138" s="27"/>
       <c r="E138" s="9"/>
     </row>
     <row r="139" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B139" s="7"/>
+      <c r="B139" s="27"/>
       <c r="E139" s="12"/>
     </row>
     <row r="140" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B140" s="7"/>
+      <c r="B140" s="27"/>
       <c r="C140" s="8"/>
       <c r="E140" s="9"/>
     </row>
     <row r="141" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B141" s="10"/>
+      <c r="B141" s="28"/>
       <c r="C141" s="8"/>
       <c r="E141" s="9"/>
       <c r="F141" s="22"/>
     </row>
     <row r="142" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B142" s="7"/>
+      <c r="B142" s="27"/>
       <c r="E142" s="9"/>
     </row>
     <row r="143" spans="2:6" x14ac:dyDescent="0.25">
@@ -1419,67 +1448,67 @@
       <c r="E143" s="9"/>
     </row>
     <row r="144" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B144" s="10"/>
+      <c r="B144" s="28"/>
       <c r="C144" s="8"/>
       <c r="E144" s="9"/>
     </row>
     <row r="145" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B145" s="7"/>
+      <c r="B145" s="27"/>
       <c r="C145" s="8"/>
       <c r="E145" s="12"/>
     </row>
     <row r="146" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B146" s="10"/>
+      <c r="B146" s="28"/>
       <c r="C146" s="8"/>
       <c r="E146" s="9"/>
     </row>
     <row r="147" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B147" s="7"/>
+      <c r="B147" s="27"/>
       <c r="C147" s="8"/>
       <c r="E147" s="9"/>
     </row>
     <row r="148" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B148" s="7"/>
+      <c r="B148" s="27"/>
       <c r="C148" s="8"/>
       <c r="E148" s="9"/>
     </row>
     <row r="149" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B149" s="7"/>
+      <c r="B149" s="27"/>
       <c r="D149" s="17"/>
       <c r="E149" s="9"/>
     </row>
     <row r="150" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B150" s="7"/>
+      <c r="B150" s="27"/>
       <c r="C150" s="8"/>
       <c r="E150" s="9"/>
     </row>
     <row r="151" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B151" s="7"/>
+      <c r="B151" s="27"/>
       <c r="C151" s="8"/>
       <c r="E151" s="9"/>
     </row>
     <row r="152" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B152" s="7"/>
+      <c r="B152" s="27"/>
       <c r="C152" s="8"/>
       <c r="E152" s="9"/>
       <c r="F152" s="22"/>
     </row>
     <row r="153" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B153" s="7"/>
+      <c r="B153" s="27"/>
       <c r="C153" s="8"/>
       <c r="E153" s="9"/>
       <c r="F153" s="24"/>
     </row>
     <row r="154" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B154" s="7"/>
+      <c r="B154" s="27"/>
       <c r="E154" s="9"/>
     </row>
     <row r="155" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B155" s="10"/>
+      <c r="B155" s="28"/>
       <c r="C155" s="8"/>
     </row>
     <row r="156" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B156" s="7"/>
+      <c r="B156" s="27"/>
       <c r="C156" s="8"/>
       <c r="E156" s="9"/>
     </row>
@@ -1488,63 +1517,63 @@
       <c r="E157" s="9"/>
     </row>
     <row r="158" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B158" s="7"/>
+      <c r="B158" s="27"/>
       <c r="C158" s="8"/>
       <c r="E158" s="9"/>
     </row>
     <row r="159" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B159" s="7"/>
+      <c r="B159" s="27"/>
       <c r="C159" s="8"/>
     </row>
     <row r="160" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B160" s="7"/>
+      <c r="B160" s="27"/>
       <c r="C160" s="8"/>
       <c r="E160" s="9"/>
     </row>
     <row r="161" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B161" s="7"/>
+      <c r="B161" s="27"/>
       <c r="C161" s="8"/>
       <c r="E161" s="12"/>
       <c r="F161" s="22"/>
     </row>
     <row r="162" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B162" s="7"/>
+      <c r="B162" s="27"/>
       <c r="C162" s="8"/>
       <c r="E162" s="9"/>
       <c r="F162" s="24"/>
     </row>
     <row r="163" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B163" s="7"/>
+      <c r="B163" s="27"/>
       <c r="E163" s="9"/>
     </row>
     <row r="164" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B164" s="7"/>
+      <c r="B164" s="27"/>
       <c r="C164" s="8"/>
       <c r="E164" s="9"/>
     </row>
     <row r="165" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B165" s="7"/>
+      <c r="B165" s="27"/>
       <c r="D165" s="16"/>
       <c r="E165" s="9"/>
     </row>
     <row r="166" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B166" s="7"/>
+      <c r="B166" s="27"/>
       <c r="D166" s="16"/>
       <c r="E166" s="9"/>
     </row>
     <row r="167" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B167" s="7"/>
+      <c r="B167" s="27"/>
       <c r="C167" s="8"/>
       <c r="D167" s="16"/>
       <c r="E167" s="12"/>
     </row>
     <row r="168" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B168" s="10"/>
+      <c r="B168" s="28"/>
       <c r="D168" s="16"/>
       <c r="E168" s="9"/>
     </row>
     <row r="169" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B169" s="7"/>
+      <c r="B169" s="27"/>
       <c r="D169" s="16"/>
       <c r="E169" s="9"/>
     </row>
@@ -1555,32 +1584,32 @@
       <c r="F170" s="22"/>
     </row>
     <row r="171" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B171" s="7"/>
+      <c r="B171" s="27"/>
       <c r="C171" s="8"/>
       <c r="E171" s="9"/>
       <c r="F171" s="24"/>
     </row>
     <row r="172" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B172" s="7"/>
+      <c r="B172" s="27"/>
       <c r="C172" s="8"/>
       <c r="E172" s="9"/>
     </row>
     <row r="173" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B173" s="7"/>
+      <c r="B173" s="27"/>
       <c r="C173" s="8"/>
       <c r="E173" s="9"/>
     </row>
     <row r="174" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B174" s="7"/>
+      <c r="B174" s="27"/>
       <c r="E174" s="9"/>
     </row>
     <row r="175" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B175" s="10"/>
+      <c r="B175" s="28"/>
       <c r="C175" s="8"/>
       <c r="E175" s="12"/>
     </row>
     <row r="176" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B176" s="7"/>
+      <c r="B176" s="27"/>
       <c r="C176" s="8"/>
       <c r="E176" s="9"/>
     </row>
@@ -1588,16 +1617,16 @@
       <c r="C177" s="8"/>
     </row>
     <row r="178" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B178" s="7"/>
+      <c r="B178" s="27"/>
       <c r="E178" s="9"/>
     </row>
     <row r="179" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B179" s="10"/>
+      <c r="B179" s="28"/>
       <c r="E179" s="9"/>
       <c r="F179" s="24"/>
     </row>
     <row r="180" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B180" s="7"/>
+      <c r="B180" s="27"/>
       <c r="C180" s="8"/>
       <c r="E180" s="12"/>
     </row>
@@ -1606,17 +1635,17 @@
       <c r="E181" s="9"/>
     </row>
     <row r="182" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B182" s="7"/>
+      <c r="B182" s="27"/>
       <c r="C182" s="8"/>
       <c r="E182" s="9"/>
     </row>
     <row r="183" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B183" s="10"/>
+      <c r="B183" s="28"/>
       <c r="C183" s="8"/>
       <c r="E183" s="9"/>
     </row>
     <row r="184" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B184" s="7"/>
+      <c r="B184" s="27"/>
       <c r="C184" s="8"/>
       <c r="E184" s="9"/>
       <c r="F184" s="22"/>
@@ -1626,7 +1655,7 @@
       <c r="F185" s="24"/>
     </row>
     <row r="186" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B186" s="7"/>
+      <c r="B186" s="27"/>
       <c r="C186" s="8"/>
       <c r="E186" s="9"/>
     </row>

</xml_diff>